<commit_message>
what a wonderful day
Signed-off-by: user2 <xtd412@qq.com>
</commit_message>
<xml_diff>
--- a/0807-0813.xlsx
+++ b/0807-0813.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="69">
   <si>
     <t>日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -283,6 +283,36 @@
   </si>
   <si>
     <t>收入的阶梯型，回头制定以下</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1：读完职场书籍
+2:3次健身房
+3：消防进入日程</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>好充实的一天</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1:月总结
+2：en
+3：周会
+4：javaee
+5：职场书籍 
+6：GERRIT调试
+7：禅道 SVN gerrit针对项目管理的优劣对比。要详细
+8：项目内部梳理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1:9:00-10：00.月报书写
+2:10:00-11:30.GERRIT梳理
+3:11:30-12:00.吃饭
+4:12:00-3:00，月总结会议
+5:3:30-5:00.禅道SVN gerrit总结PPT书写
+6:5:10-6:30聚传拓展总结并发出</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -523,6 +553,30 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -541,35 +595,11 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -854,7 +884,7 @@
   <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="99.95" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -877,70 +907,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="33" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="11"/>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="35" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="12"/>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="G1" s="37" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="13"/>
-      <c r="I1" s="36" t="s">
+      <c r="I1" s="26" t="s">
         <v>12</v>
       </c>
       <c r="J1" s="14"/>
-      <c r="K1" s="38" t="s">
+      <c r="K1" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="29" t="s">
+      <c r="L1" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="29" t="s">
+      <c r="M1" s="30" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="1" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="24"/>
-      <c r="B2" s="26"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="34"/>
       <c r="C2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="28"/>
+      <c r="D2" s="36"/>
       <c r="E2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="30"/>
-      <c r="G2" s="32"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="38"/>
       <c r="H2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="37"/>
+      <c r="I2" s="27"/>
       <c r="J2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="33"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="23"/>
     </row>
     <row r="3" spans="1:14" s="1" customFormat="1" ht="258.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
         <v>42954</v>
       </c>
-      <c r="B3" s="16"/>
+      <c r="B3" s="16" t="s">
+        <v>67</v>
+      </c>
       <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="3"/>
+      <c r="D3" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="F3" s="16"/>
       <c r="G3" s="16"/>
       <c r="H3" s="4"/>
@@ -948,8 +984,10 @@
       <c r="J3" s="16"/>
       <c r="K3" s="16"/>
       <c r="L3" s="16"/>
-      <c r="M3" s="33"/>
-      <c r="N3" s="34"/>
+      <c r="M3" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="N3" s="24"/>
     </row>
     <row r="4" spans="1:14" s="1" customFormat="1" ht="144.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
@@ -966,8 +1004,8 @@
       <c r="J4" s="5"/>
       <c r="K4" s="17"/>
       <c r="L4" s="16"/>
-      <c r="M4" s="34"/>
-      <c r="N4" s="35"/>
+      <c r="M4" s="24"/>
+      <c r="N4" s="25"/>
     </row>
     <row r="5" spans="1:14" s="1" customFormat="1" ht="141" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
@@ -984,7 +1022,7 @@
       <c r="J5" s="16"/>
       <c r="K5" s="16"/>
       <c r="L5" s="16"/>
-      <c r="M5" s="34"/>
+      <c r="M5" s="24"/>
     </row>
     <row r="6" spans="1:14" s="1" customFormat="1" ht="155.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
@@ -1001,7 +1039,7 @@
       <c r="J6" s="16"/>
       <c r="K6" s="16"/>
       <c r="L6" s="16"/>
-      <c r="M6" s="34"/>
+      <c r="M6" s="24"/>
     </row>
     <row r="7" spans="1:14" s="1" customFormat="1" ht="219.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
@@ -1018,7 +1056,7 @@
       <c r="J7" s="16"/>
       <c r="K7" s="16"/>
       <c r="L7" s="16"/>
-      <c r="M7" s="34"/>
+      <c r="M7" s="24"/>
     </row>
     <row r="8" spans="1:14" s="1" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
@@ -1035,7 +1073,7 @@
       <c r="J8" s="16"/>
       <c r="K8" s="16"/>
       <c r="L8" s="16"/>
-      <c r="M8" s="34"/>
+      <c r="M8" s="24"/>
     </row>
     <row r="9" spans="1:14" s="1" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
@@ -1052,7 +1090,7 @@
       <c r="J9" s="16"/>
       <c r="K9" s="16"/>
       <c r="L9" s="16"/>
-      <c r="M9" s="35"/>
+      <c r="M9" s="25"/>
     </row>
     <row r="10" spans="1:14" s="1" customFormat="1" ht="168" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7"/>
@@ -1067,7 +1105,7 @@
       <c r="J10" s="16"/>
       <c r="K10" s="16"/>
       <c r="L10" s="16"/>
-      <c r="M10" s="33"/>
+      <c r="M10" s="23"/>
     </row>
     <row r="11" spans="1:14" s="1" customFormat="1" ht="171.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7"/>
@@ -1082,7 +1120,7 @@
       <c r="J11" s="16"/>
       <c r="K11" s="16"/>
       <c r="L11" s="16"/>
-      <c r="M11" s="34"/>
+      <c r="M11" s="24"/>
     </row>
     <row r="12" spans="1:14" s="1" customFormat="1" ht="147.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="7"/>
@@ -1097,7 +1135,7 @@
       <c r="J12" s="16"/>
       <c r="K12" s="16"/>
       <c r="L12" s="16"/>
-      <c r="M12" s="34"/>
+      <c r="M12" s="24"/>
     </row>
     <row r="13" spans="1:14" s="1" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7"/>
@@ -1112,7 +1150,7 @@
       <c r="J13" s="16"/>
       <c r="K13" s="16"/>
       <c r="L13" s="16"/>
-      <c r="M13" s="34"/>
+      <c r="M13" s="24"/>
     </row>
     <row r="14" spans="1:14" s="1" customFormat="1" ht="129.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="7"/>
@@ -1127,7 +1165,7 @@
       <c r="J14" s="16"/>
       <c r="K14" s="16"/>
       <c r="L14" s="16"/>
-      <c r="M14" s="35"/>
+      <c r="M14" s="25"/>
     </row>
     <row r="15" spans="1:14" s="1" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="7"/>
@@ -1172,7 +1210,7 @@
       <c r="J17" s="16"/>
       <c r="K17" s="16"/>
       <c r="L17" s="16"/>
-      <c r="M17" s="33"/>
+      <c r="M17" s="23"/>
     </row>
     <row r="18" spans="1:13" s="1" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="7"/>
@@ -1187,7 +1225,7 @@
       <c r="J18" s="16"/>
       <c r="K18" s="16"/>
       <c r="L18" s="16"/>
-      <c r="M18" s="34"/>
+      <c r="M18" s="24"/>
     </row>
     <row r="19" spans="1:13" s="1" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="7"/>
@@ -1202,7 +1240,7 @@
       <c r="J19" s="16"/>
       <c r="K19" s="16"/>
       <c r="L19" s="16"/>
-      <c r="M19" s="34"/>
+      <c r="M19" s="24"/>
     </row>
     <row r="20" spans="1:13" s="1" customFormat="1" ht="174.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="7"/>
@@ -1217,7 +1255,7 @@
       <c r="J20" s="16"/>
       <c r="K20" s="16"/>
       <c r="L20" s="16"/>
-      <c r="M20" s="34"/>
+      <c r="M20" s="24"/>
     </row>
     <row r="21" spans="1:13" s="1" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="7"/>
@@ -1232,7 +1270,7 @@
       <c r="J21" s="16"/>
       <c r="K21" s="16"/>
       <c r="L21" s="16"/>
-      <c r="M21" s="34"/>
+      <c r="M21" s="24"/>
     </row>
     <row r="22" spans="1:13" s="1" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="7"/>
@@ -1247,7 +1285,7 @@
       <c r="J22" s="16"/>
       <c r="K22" s="16"/>
       <c r="L22" s="16"/>
-      <c r="M22" s="34"/>
+      <c r="M22" s="24"/>
     </row>
     <row r="23" spans="1:13" s="1" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="7"/>
@@ -1262,7 +1300,7 @@
       <c r="J23" s="16"/>
       <c r="K23" s="16"/>
       <c r="L23" s="16"/>
-      <c r="M23" s="35"/>
+      <c r="M23" s="25"/>
     </row>
     <row r="24" spans="1:13" s="1" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="7"/>
@@ -1401,6 +1439,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
     <mergeCell ref="M17:M23"/>
     <mergeCell ref="N2:N4"/>
     <mergeCell ref="I1:I2"/>
@@ -1409,11 +1452,6 @@
     <mergeCell ref="M3:M9"/>
     <mergeCell ref="M10:M14"/>
     <mergeCell ref="M1:M2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add sth have done today
Signed-off-by: user2 <xtd412@qq.com>
</commit_message>
<xml_diff>
--- a/0807-0813.xlsx
+++ b/0807-0813.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="73">
   <si>
     <t>日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -315,12 +315,67 @@
 6:5:10-6:30聚传拓展总结并发出</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <r>
+      <t>1：聚传开发者拓展
+2：职场书籍
+3：javaee</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4：GERRIT 包的获取，
+5：项目内部梳理</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1 9:00-9:30，聚传拓展任务
+2 9:30-11:00,javaee
+3:2:00-2:30.职场书籍
+4:3:00-5:00.GERRIT的环境配置与调试
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1：三种工具对比表格文档制作
+2：内部项目梳理
+3：javaee
+4：GERRIT调试
+5：买帐篷、充气垫
+6：职场书籍</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1:9:00-10:30，三种工具比较
+2：10:40-11：30.项目书籍</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -369,6 +424,15 @@
     </font>
     <font>
       <sz val="24"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="等线"/>
       <family val="3"/>
@@ -553,30 +617,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -595,11 +635,35 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -883,8 +947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="99.95" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -907,61 +971,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="25" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="11"/>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="27" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="12"/>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="37" t="s">
+      <c r="G1" s="31" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="13"/>
-      <c r="I1" s="26" t="s">
+      <c r="I1" s="36" t="s">
         <v>12</v>
       </c>
       <c r="J1" s="14"/>
-      <c r="K1" s="28" t="s">
+      <c r="K1" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="30" t="s">
+      <c r="L1" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="30" t="s">
+      <c r="M1" s="29" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="1" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="32"/>
-      <c r="B2" s="34"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="26"/>
       <c r="C2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="36"/>
+      <c r="D2" s="28"/>
       <c r="E2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="29"/>
-      <c r="G2" s="38"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="32"/>
       <c r="H2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="27"/>
+      <c r="I2" s="37"/>
       <c r="J2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="23"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="33"/>
     </row>
     <row r="3" spans="1:14" s="1" customFormat="1" ht="258.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
@@ -984,18 +1048,22 @@
       <c r="J3" s="16"/>
       <c r="K3" s="16"/>
       <c r="L3" s="16"/>
-      <c r="M3" s="23" t="s">
+      <c r="M3" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="N3" s="24"/>
+      <c r="N3" s="34"/>
     </row>
     <row r="4" spans="1:14" s="1" customFormat="1" ht="144.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
         <v>42955</v>
       </c>
-      <c r="B4" s="16"/>
+      <c r="B4" s="16" t="s">
+        <v>69</v>
+      </c>
       <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
+      <c r="D4" s="16" t="s">
+        <v>70</v>
+      </c>
       <c r="E4" s="3"/>
       <c r="F4" s="16"/>
       <c r="G4" s="16"/>
@@ -1004,16 +1072,20 @@
       <c r="J4" s="5"/>
       <c r="K4" s="17"/>
       <c r="L4" s="16"/>
-      <c r="M4" s="24"/>
-      <c r="N4" s="25"/>
+      <c r="M4" s="34"/>
+      <c r="N4" s="35"/>
     </row>
     <row r="5" spans="1:14" s="1" customFormat="1" ht="141" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
         <v>42956</v>
       </c>
-      <c r="B5" s="16"/>
+      <c r="B5" s="16" t="s">
+        <v>71</v>
+      </c>
       <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
+      <c r="D5" s="16" t="s">
+        <v>72</v>
+      </c>
       <c r="E5" s="16"/>
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
@@ -1022,7 +1094,7 @@
       <c r="J5" s="16"/>
       <c r="K5" s="16"/>
       <c r="L5" s="16"/>
-      <c r="M5" s="24"/>
+      <c r="M5" s="34"/>
     </row>
     <row r="6" spans="1:14" s="1" customFormat="1" ht="155.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
@@ -1039,7 +1111,7 @@
       <c r="J6" s="16"/>
       <c r="K6" s="16"/>
       <c r="L6" s="16"/>
-      <c r="M6" s="24"/>
+      <c r="M6" s="34"/>
     </row>
     <row r="7" spans="1:14" s="1" customFormat="1" ht="219.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
@@ -1056,7 +1128,7 @@
       <c r="J7" s="16"/>
       <c r="K7" s="16"/>
       <c r="L7" s="16"/>
-      <c r="M7" s="24"/>
+      <c r="M7" s="34"/>
     </row>
     <row r="8" spans="1:14" s="1" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
@@ -1073,7 +1145,7 @@
       <c r="J8" s="16"/>
       <c r="K8" s="16"/>
       <c r="L8" s="16"/>
-      <c r="M8" s="24"/>
+      <c r="M8" s="34"/>
     </row>
     <row r="9" spans="1:14" s="1" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
@@ -1090,7 +1162,7 @@
       <c r="J9" s="16"/>
       <c r="K9" s="16"/>
       <c r="L9" s="16"/>
-      <c r="M9" s="25"/>
+      <c r="M9" s="35"/>
     </row>
     <row r="10" spans="1:14" s="1" customFormat="1" ht="168" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7"/>
@@ -1105,7 +1177,7 @@
       <c r="J10" s="16"/>
       <c r="K10" s="16"/>
       <c r="L10" s="16"/>
-      <c r="M10" s="23"/>
+      <c r="M10" s="33"/>
     </row>
     <row r="11" spans="1:14" s="1" customFormat="1" ht="171.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7"/>
@@ -1120,7 +1192,7 @@
       <c r="J11" s="16"/>
       <c r="K11" s="16"/>
       <c r="L11" s="16"/>
-      <c r="M11" s="24"/>
+      <c r="M11" s="34"/>
     </row>
     <row r="12" spans="1:14" s="1" customFormat="1" ht="147.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="7"/>
@@ -1135,7 +1207,7 @@
       <c r="J12" s="16"/>
       <c r="K12" s="16"/>
       <c r="L12" s="16"/>
-      <c r="M12" s="24"/>
+      <c r="M12" s="34"/>
     </row>
     <row r="13" spans="1:14" s="1" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7"/>
@@ -1150,7 +1222,7 @@
       <c r="J13" s="16"/>
       <c r="K13" s="16"/>
       <c r="L13" s="16"/>
-      <c r="M13" s="24"/>
+      <c r="M13" s="34"/>
     </row>
     <row r="14" spans="1:14" s="1" customFormat="1" ht="129.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="7"/>
@@ -1165,7 +1237,7 @@
       <c r="J14" s="16"/>
       <c r="K14" s="16"/>
       <c r="L14" s="16"/>
-      <c r="M14" s="25"/>
+      <c r="M14" s="35"/>
     </row>
     <row r="15" spans="1:14" s="1" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="7"/>
@@ -1210,7 +1282,7 @@
       <c r="J17" s="16"/>
       <c r="K17" s="16"/>
       <c r="L17" s="16"/>
-      <c r="M17" s="23"/>
+      <c r="M17" s="33"/>
     </row>
     <row r="18" spans="1:13" s="1" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="7"/>
@@ -1225,7 +1297,7 @@
       <c r="J18" s="16"/>
       <c r="K18" s="16"/>
       <c r="L18" s="16"/>
-      <c r="M18" s="24"/>
+      <c r="M18" s="34"/>
     </row>
     <row r="19" spans="1:13" s="1" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="7"/>
@@ -1240,7 +1312,7 @@
       <c r="J19" s="16"/>
       <c r="K19" s="16"/>
       <c r="L19" s="16"/>
-      <c r="M19" s="24"/>
+      <c r="M19" s="34"/>
     </row>
     <row r="20" spans="1:13" s="1" customFormat="1" ht="174.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="7"/>
@@ -1255,7 +1327,7 @@
       <c r="J20" s="16"/>
       <c r="K20" s="16"/>
       <c r="L20" s="16"/>
-      <c r="M20" s="24"/>
+      <c r="M20" s="34"/>
     </row>
     <row r="21" spans="1:13" s="1" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="7"/>
@@ -1270,7 +1342,7 @@
       <c r="J21" s="16"/>
       <c r="K21" s="16"/>
       <c r="L21" s="16"/>
-      <c r="M21" s="24"/>
+      <c r="M21" s="34"/>
     </row>
     <row r="22" spans="1:13" s="1" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="7"/>
@@ -1285,7 +1357,7 @@
       <c r="J22" s="16"/>
       <c r="K22" s="16"/>
       <c r="L22" s="16"/>
-      <c r="M22" s="24"/>
+      <c r="M22" s="34"/>
     </row>
     <row r="23" spans="1:13" s="1" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="7"/>
@@ -1300,7 +1372,7 @@
       <c r="J23" s="16"/>
       <c r="K23" s="16"/>
       <c r="L23" s="16"/>
-      <c r="M23" s="25"/>
+      <c r="M23" s="35"/>
     </row>
     <row r="24" spans="1:13" s="1" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="7"/>
@@ -1439,11 +1511,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
     <mergeCell ref="M17:M23"/>
     <mergeCell ref="N2:N4"/>
     <mergeCell ref="I1:I2"/>
@@ -1452,6 +1519,11 @@
     <mergeCell ref="M3:M9"/>
     <mergeCell ref="M10:M14"/>
     <mergeCell ref="M1:M2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>